<commit_message>
micro service partiellement ok
</commit_message>
<xml_diff>
--- a/generated_files/user_predict.xlsx
+++ b/generated_files/user_predict.xlsx
@@ -500,56 +500,56 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>27.7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>724</v>
+      </c>
+      <c r="I2" t="n">
+        <v>25</v>
+      </c>
+      <c r="J2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>477218.363636364</v>
-      </c>
-      <c r="I2" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="J2" t="n">
-        <v>8000</v>
-      </c>
       <c r="K2" t="n">
-        <v>477</v>
+        <v>61</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>SAN PEDRO</t>
+          <t>baby</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>masculin</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>SERV.TECH.ING/ARCHIT</t>
+          <t>code</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>GRP</t>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>